<commit_message>
WIN-CP ACTUALIZACION ENTREGABLE 2
</commit_message>
<xml_diff>
--- a/WIN/Librería de Trabajo/Gestión de Proyecto/WIN-CP.xlsx
+++ b/WIN/Librería de Trabajo/Gestión de Proyecto/WIN-CP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\Cinco-Inc\WIN\Librería de Trabajo\Gestión de Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Documents\Ciclo VII\Gestión de la Configuración\Proyecto De Curso\Cinco-Inc\WIN\Librería de Trabajo\Gestión de Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
   <si>
     <t>Work In Nestle</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>Implementar CU5</t>
+  </si>
+  <si>
+    <t>DQ, DO, RP,JQ,AO</t>
+  </si>
+  <si>
+    <t>Entregado</t>
   </si>
 </sst>
 </file>
@@ -732,6 +738,9 @@
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -740,9 +749,6 @@
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1123,7 +1129,7 @@
   <dimension ref="A1:DX1048576"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="AN15" sqref="AN15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1150,8 +1156,8 @@
       <c r="D1" s="62"/>
       <c r="E1" s="72"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
       <c r="I1" s="3"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -1525,7 +1531,7 @@
       </c>
       <c r="H4" s="10">
         <f ca="1">TODAY()</f>
-        <v>42476</v>
+        <v>42490</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="4"/>
@@ -1759,11 +1765,11 @@
       <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="76" t="s">
+      <c r="C6" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -1881,10 +1887,10 @@
       <c r="B7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="77">
+      <c r="C7" s="78">
         <v>42462</v>
       </c>
-      <c r="D7" s="77"/>
+      <c r="D7" s="78"/>
       <c r="E7" s="73"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -2527,176 +2533,176 @@
         <v>59</v>
       </c>
       <c r="I9" s="21"/>
-      <c r="J9" s="78">
+      <c r="J9" s="75">
         <f>J8</f>
         <v>42462</v>
       </c>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78"/>
-      <c r="N9" s="78"/>
-      <c r="O9" s="78"/>
-      <c r="P9" s="78"/>
-      <c r="Q9" s="78">
+      <c r="K9" s="75"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="75">
         <f>Q8</f>
         <v>42469</v>
       </c>
-      <c r="R9" s="78"/>
-      <c r="S9" s="78"/>
-      <c r="T9" s="78"/>
-      <c r="U9" s="78"/>
-      <c r="V9" s="78"/>
-      <c r="W9" s="78"/>
-      <c r="X9" s="78">
+      <c r="R9" s="75"/>
+      <c r="S9" s="75"/>
+      <c r="T9" s="75"/>
+      <c r="U9" s="75"/>
+      <c r="V9" s="75"/>
+      <c r="W9" s="75"/>
+      <c r="X9" s="75">
         <f>X8</f>
         <v>42476</v>
       </c>
-      <c r="Y9" s="78"/>
-      <c r="Z9" s="78"/>
-      <c r="AA9" s="78"/>
-      <c r="AB9" s="78"/>
-      <c r="AC9" s="78"/>
-      <c r="AD9" s="78"/>
-      <c r="AE9" s="78">
+      <c r="Y9" s="75"/>
+      <c r="Z9" s="75"/>
+      <c r="AA9" s="75"/>
+      <c r="AB9" s="75"/>
+      <c r="AC9" s="75"/>
+      <c r="AD9" s="75"/>
+      <c r="AE9" s="75">
         <f>AE8</f>
         <v>42483</v>
       </c>
-      <c r="AF9" s="78"/>
-      <c r="AG9" s="78"/>
-      <c r="AH9" s="78"/>
-      <c r="AI9" s="78"/>
-      <c r="AJ9" s="78"/>
-      <c r="AK9" s="78"/>
-      <c r="AL9" s="78">
+      <c r="AF9" s="75"/>
+      <c r="AG9" s="75"/>
+      <c r="AH9" s="75"/>
+      <c r="AI9" s="75"/>
+      <c r="AJ9" s="75"/>
+      <c r="AK9" s="75"/>
+      <c r="AL9" s="75">
         <f>AL8</f>
         <v>42490</v>
       </c>
-      <c r="AM9" s="78"/>
-      <c r="AN9" s="78"/>
-      <c r="AO9" s="78"/>
-      <c r="AP9" s="78"/>
-      <c r="AQ9" s="78"/>
-      <c r="AR9" s="78"/>
-      <c r="AS9" s="78">
+      <c r="AM9" s="75"/>
+      <c r="AN9" s="75"/>
+      <c r="AO9" s="75"/>
+      <c r="AP9" s="75"/>
+      <c r="AQ9" s="75"/>
+      <c r="AR9" s="75"/>
+      <c r="AS9" s="75">
         <f>AS8</f>
         <v>42497</v>
       </c>
-      <c r="AT9" s="78"/>
-      <c r="AU9" s="78"/>
-      <c r="AV9" s="78"/>
-      <c r="AW9" s="78"/>
-      <c r="AX9" s="78"/>
-      <c r="AY9" s="78"/>
-      <c r="AZ9" s="78">
+      <c r="AT9" s="75"/>
+      <c r="AU9" s="75"/>
+      <c r="AV9" s="75"/>
+      <c r="AW9" s="75"/>
+      <c r="AX9" s="75"/>
+      <c r="AY9" s="75"/>
+      <c r="AZ9" s="75">
         <f>AZ8</f>
         <v>42504</v>
       </c>
-      <c r="BA9" s="78"/>
-      <c r="BB9" s="78"/>
-      <c r="BC9" s="78"/>
-      <c r="BD9" s="78"/>
-      <c r="BE9" s="78"/>
-      <c r="BF9" s="78"/>
-      <c r="BG9" s="78">
+      <c r="BA9" s="75"/>
+      <c r="BB9" s="75"/>
+      <c r="BC9" s="75"/>
+      <c r="BD9" s="75"/>
+      <c r="BE9" s="75"/>
+      <c r="BF9" s="75"/>
+      <c r="BG9" s="75">
         <f>BG8</f>
         <v>42511</v>
       </c>
-      <c r="BH9" s="78"/>
-      <c r="BI9" s="78"/>
-      <c r="BJ9" s="78"/>
-      <c r="BK9" s="78"/>
-      <c r="BL9" s="78"/>
-      <c r="BM9" s="78"/>
-      <c r="BN9" s="78">
+      <c r="BH9" s="75"/>
+      <c r="BI9" s="75"/>
+      <c r="BJ9" s="75"/>
+      <c r="BK9" s="75"/>
+      <c r="BL9" s="75"/>
+      <c r="BM9" s="75"/>
+      <c r="BN9" s="75">
         <f>BN8</f>
         <v>42518</v>
       </c>
-      <c r="BO9" s="78"/>
-      <c r="BP9" s="78"/>
-      <c r="BQ9" s="78"/>
-      <c r="BR9" s="78"/>
-      <c r="BS9" s="78"/>
-      <c r="BT9" s="78"/>
-      <c r="BU9" s="78">
+      <c r="BO9" s="75"/>
+      <c r="BP9" s="75"/>
+      <c r="BQ9" s="75"/>
+      <c r="BR9" s="75"/>
+      <c r="BS9" s="75"/>
+      <c r="BT9" s="75"/>
+      <c r="BU9" s="75">
         <f>BU8</f>
         <v>42525</v>
       </c>
-      <c r="BV9" s="78"/>
-      <c r="BW9" s="78"/>
-      <c r="BX9" s="78"/>
-      <c r="BY9" s="78"/>
-      <c r="BZ9" s="78"/>
-      <c r="CA9" s="78"/>
-      <c r="CB9" s="78">
+      <c r="BV9" s="75"/>
+      <c r="BW9" s="75"/>
+      <c r="BX9" s="75"/>
+      <c r="BY9" s="75"/>
+      <c r="BZ9" s="75"/>
+      <c r="CA9" s="75"/>
+      <c r="CB9" s="75">
         <f>CB8</f>
         <v>42532</v>
       </c>
-      <c r="CC9" s="78"/>
-      <c r="CD9" s="78"/>
-      <c r="CE9" s="78"/>
-      <c r="CF9" s="78"/>
-      <c r="CG9" s="78"/>
-      <c r="CH9" s="78"/>
-      <c r="CI9" s="78">
+      <c r="CC9" s="75"/>
+      <c r="CD9" s="75"/>
+      <c r="CE9" s="75"/>
+      <c r="CF9" s="75"/>
+      <c r="CG9" s="75"/>
+      <c r="CH9" s="75"/>
+      <c r="CI9" s="75">
         <f>CI8</f>
         <v>42539</v>
       </c>
-      <c r="CJ9" s="78"/>
-      <c r="CK9" s="78"/>
-      <c r="CL9" s="78"/>
-      <c r="CM9" s="78"/>
-      <c r="CN9" s="78"/>
-      <c r="CO9" s="78"/>
-      <c r="CP9" s="78">
+      <c r="CJ9" s="75"/>
+      <c r="CK9" s="75"/>
+      <c r="CL9" s="75"/>
+      <c r="CM9" s="75"/>
+      <c r="CN9" s="75"/>
+      <c r="CO9" s="75"/>
+      <c r="CP9" s="75">
         <f>CP8</f>
         <v>42546</v>
       </c>
-      <c r="CQ9" s="78"/>
-      <c r="CR9" s="78"/>
-      <c r="CS9" s="78"/>
-      <c r="CT9" s="78"/>
-      <c r="CU9" s="78"/>
-      <c r="CV9" s="78"/>
-      <c r="CW9" s="78">
+      <c r="CQ9" s="75"/>
+      <c r="CR9" s="75"/>
+      <c r="CS9" s="75"/>
+      <c r="CT9" s="75"/>
+      <c r="CU9" s="75"/>
+      <c r="CV9" s="75"/>
+      <c r="CW9" s="75">
         <f>CW8</f>
         <v>42553</v>
       </c>
-      <c r="CX9" s="78"/>
-      <c r="CY9" s="78"/>
-      <c r="CZ9" s="78"/>
-      <c r="DA9" s="78"/>
-      <c r="DB9" s="78"/>
-      <c r="DC9" s="78"/>
-      <c r="DD9" s="78">
+      <c r="CX9" s="75"/>
+      <c r="CY9" s="75"/>
+      <c r="CZ9" s="75"/>
+      <c r="DA9" s="75"/>
+      <c r="DB9" s="75"/>
+      <c r="DC9" s="75"/>
+      <c r="DD9" s="75">
         <f>DD8</f>
         <v>42560</v>
       </c>
-      <c r="DE9" s="78"/>
-      <c r="DF9" s="78"/>
-      <c r="DG9" s="78"/>
-      <c r="DH9" s="78"/>
-      <c r="DI9" s="78"/>
-      <c r="DJ9" s="78"/>
-      <c r="DK9" s="78">
+      <c r="DE9" s="75"/>
+      <c r="DF9" s="75"/>
+      <c r="DG9" s="75"/>
+      <c r="DH9" s="75"/>
+      <c r="DI9" s="75"/>
+      <c r="DJ9" s="75"/>
+      <c r="DK9" s="75">
         <f>DK8</f>
         <v>42567</v>
       </c>
-      <c r="DL9" s="78"/>
-      <c r="DM9" s="78"/>
-      <c r="DN9" s="78"/>
-      <c r="DO9" s="78"/>
-      <c r="DP9" s="78"/>
-      <c r="DQ9" s="78"/>
-      <c r="DR9" s="78">
+      <c r="DL9" s="75"/>
+      <c r="DM9" s="75"/>
+      <c r="DN9" s="75"/>
+      <c r="DO9" s="75"/>
+      <c r="DP9" s="75"/>
+      <c r="DQ9" s="75"/>
+      <c r="DR9" s="75">
         <f>DR8</f>
         <v>42574</v>
       </c>
-      <c r="DS9" s="78"/>
-      <c r="DT9" s="78"/>
-      <c r="DU9" s="78"/>
-      <c r="DV9" s="78"/>
-      <c r="DW9" s="78"/>
-      <c r="DX9" s="78"/>
+      <c r="DS9" s="75"/>
+      <c r="DT9" s="75"/>
+      <c r="DU9" s="75"/>
+      <c r="DV9" s="75"/>
+      <c r="DW9" s="75"/>
+      <c r="DX9" s="75"/>
     </row>
     <row r="10" spans="1:128" x14ac:dyDescent="0.2">
       <c r="A10" s="22">
@@ -3152,13 +3158,20 @@
       <c r="C13" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="27" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
+      <c r="D13" s="67">
+        <v>42506</v>
+      </c>
+      <c r="E13" s="67">
+        <v>42512</v>
+      </c>
+      <c r="F13" s="39">
+        <v>7</v>
+      </c>
+      <c r="G13" s="40">
+        <v>1</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="I13" s="41"/>
       <c r="J13" s="41"/>
@@ -3175,13 +3188,13 @@
       <c r="U13" s="41"/>
       <c r="V13" s="41"/>
       <c r="W13" s="41"/>
-      <c r="X13" s="41"/>
-      <c r="Y13" s="41"/>
-      <c r="Z13" s="41"/>
-      <c r="AA13" s="41"/>
-      <c r="AB13" s="41"/>
-      <c r="AC13" s="41"/>
-      <c r="AD13" s="41"/>
+      <c r="X13" s="29"/>
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="29"/>
+      <c r="AA13" s="29"/>
+      <c r="AB13" s="29"/>
+      <c r="AC13" s="29"/>
+      <c r="AD13" s="29"/>
       <c r="AE13" s="41"/>
       <c r="AF13" s="41"/>
       <c r="AG13" s="41"/>
@@ -3289,14 +3302,23 @@
       <c r="B14" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="27" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
+      <c r="C14" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="67">
+        <v>42506</v>
+      </c>
+      <c r="E14" s="67">
+        <v>42511</v>
+      </c>
+      <c r="F14" s="33">
+        <v>5</v>
+      </c>
+      <c r="G14" s="34">
+        <v>1</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="I14" s="35"/>
       <c r="J14" s="35"/>
@@ -3313,12 +3335,12 @@
       <c r="U14" s="35"/>
       <c r="V14" s="35"/>
       <c r="W14" s="35"/>
-      <c r="X14" s="35"/>
-      <c r="Y14" s="35"/>
-      <c r="Z14" s="35"/>
-      <c r="AA14" s="35"/>
-      <c r="AB14" s="35"/>
-      <c r="AC14" s="35"/>
+      <c r="X14" s="36"/>
+      <c r="Y14" s="36"/>
+      <c r="Z14" s="36"/>
+      <c r="AA14" s="36"/>
+      <c r="AB14" s="36"/>
+      <c r="AC14" s="36"/>
       <c r="AD14" s="35"/>
       <c r="AE14" s="35"/>
       <c r="AF14" s="35"/>
@@ -3427,14 +3449,23 @@
       <c r="B15" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="27" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
+      <c r="C15" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="67">
+        <v>42511</v>
+      </c>
+      <c r="E15" s="67">
+        <v>42512</v>
+      </c>
+      <c r="F15" s="33">
+        <v>1</v>
+      </c>
+      <c r="G15" s="34">
+        <v>1</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="I15" s="35"/>
       <c r="J15" s="35"/>
@@ -3457,7 +3488,7 @@
       <c r="AA15" s="35"/>
       <c r="AB15" s="35"/>
       <c r="AC15" s="35"/>
-      <c r="AD15" s="35"/>
+      <c r="AD15" s="36"/>
       <c r="AE15" s="35"/>
       <c r="AF15" s="35"/>
       <c r="AG15" s="35"/>
@@ -9694,6 +9725,16 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="J9:P9"/>
+    <mergeCell ref="Q9:W9"/>
+    <mergeCell ref="X9:AD9"/>
+    <mergeCell ref="AE9:AK9"/>
+    <mergeCell ref="AL9:AR9"/>
+    <mergeCell ref="AS9:AY9"/>
+    <mergeCell ref="AZ9:BF9"/>
     <mergeCell ref="BG9:BM9"/>
     <mergeCell ref="BN9:BT9"/>
     <mergeCell ref="BU9:CA9"/>
@@ -9704,16 +9745,6 @@
     <mergeCell ref="CP9:CV9"/>
     <mergeCell ref="CW9:DC9"/>
     <mergeCell ref="DD9:DJ9"/>
-    <mergeCell ref="X9:AD9"/>
-    <mergeCell ref="AE9:AK9"/>
-    <mergeCell ref="AL9:AR9"/>
-    <mergeCell ref="AS9:AY9"/>
-    <mergeCell ref="AZ9:BF9"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="J9:P9"/>
-    <mergeCell ref="Q9:W9"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>